<commit_message>
Practica 4: Cree PWM con control de Duty Cicle con timer 0
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\C embebido\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE1E2AF-2BE2-49FE-A30D-5F6A464B424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1424784-2B0F-4123-B822-DD10B84995E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,10 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Duty">Hoja1!$E$4</definedName>
-    <definedName name="Fosc">Hoja1!$B$4</definedName>
-    <definedName name="Fpwm">Hoja1!$D$4</definedName>
-    <definedName name="Pre">Hoja1!$C$4</definedName>
+    <definedName name="Duty">Hoja1!$E$5</definedName>
+    <definedName name="Fosc">Hoja1!$B$5</definedName>
+    <definedName name="Fpwm">Hoja1!$D$5</definedName>
+    <definedName name="Pre">Hoja1!$C$5</definedName>
     <definedName name="Tpwm">Hoja1!$B$7</definedName>
     <definedName name="valPR2">Hoja1!$C$7</definedName>
   </definedNames>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>SE CONOCEN ESTOS DATOS</t>
   </si>
@@ -69,16 +69,50 @@
   <si>
     <t>CCPRXL:CCPXCON&lt;5:4&gt;</t>
   </si>
+  <si>
+    <t>TIMER0</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>Valor de TMR0</t>
+  </si>
+  <si>
+    <t>Pre-escaler Timer 0</t>
+  </si>
+  <si>
+    <t>Quiero una señal de 1 kHz</t>
+  </si>
+  <si>
+    <t>Frecuencia (Hz)</t>
+  </si>
+  <si>
+    <t>Periodo de cuenta (s)</t>
+  </si>
+  <si>
+    <t>Tiempo Ciclo Maquina (s)</t>
+  </si>
+  <si>
+    <t>Bits de Timer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -121,8 +155,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,8 +188,14 @@
         <bgColor rgb="FF4472C4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -376,65 +423,252 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -442,7 +676,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -664,61 +908,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E815"/>
+  <dimension ref="B1:G809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="20" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="19" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8">
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="8">
         <v>8</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C5" s="9">
         <v>16</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D5" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E5" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -732,7 +984,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <f>1/(Fpwm/1000)</f>
         <v>1000</v>
@@ -750,14 +1002,80 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="G10" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="23">
+        <v>8</v>
+      </c>
+      <c r="C12" s="22">
+        <f>4/(B12*1000000)</f>
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="E12" s="18">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="8">
+        <f>1/E12</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C14" s="26">
+        <f>(_xlfn.BITLSHIFT(1,E14))-(B14)/(C12*D12)</f>
+        <v>64536</v>
+      </c>
+      <c r="E14" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1551,28 +1869,37 @@
     <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
+      <formula>0</formula>
+      <formula>255</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
       <formula>0</formula>
       <formula>255</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,4,16"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="B5 B12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D12" xr:uid="{5825D9D1-57B3-4C3C-A12F-8A11388FAA98}">
+      <formula1>"1,2,4,8,16,32,64,128,256"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14" xr:uid="{53587E53-2A95-4374-A80D-039A9E8F71AC}">
+      <formula1>"8,16"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Practica 4: Version Final del codigo
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\C embebido\Recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\C_embebido\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1424784-2B0F-4123-B822-DD10B84995E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F900D9-27F7-4C3C-97CC-8AE3B4C9E8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -910,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G809"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -998,8 +998,8 @@
         <v>10</v>
       </c>
       <c r="E7" s="15">
-        <f>(Duty*Tpwm)/((1/Fosc)*Pre)</f>
-        <v>500</v>
+        <f>(Duty*Tpwm*Fosc)/(Pre)</f>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Practica 5: Recibimos caracteres de puerto serial a 9600 baudios
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\C_embebido\Recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Microcontroladores_PIC\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F900D9-27F7-4C3C-97CC-8AE3B4C9E8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3215DC58-BFEF-4DF0-858B-0C2617B9E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>SE CONOCEN ESTOS DATOS</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Resolucion Maxima (Bits)</t>
-  </si>
-  <si>
-    <t>F(PWM) Khz</t>
   </si>
   <si>
     <t>Duty Cicle</t>
@@ -95,6 +92,12 @@
   </si>
   <si>
     <t>Bits de Timer</t>
+  </si>
+  <si>
+    <t>F(PWM) Hz</t>
+  </si>
+  <si>
+    <t>TIMER2</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -671,12 +674,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -910,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G809"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -928,7 +945,7 @@
     <row r="1" spans="2:7" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -950,10 +967,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -964,10 +981,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="9">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="E5" s="11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -981,30 +998,30 @@
         <v>5</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
-        <f>1/(Fpwm/1000)</f>
-        <v>1000</v>
+        <f>1/Fpwm</f>
+        <v>1E-3</v>
       </c>
       <c r="C7" s="2">
-        <f>((Tpwm)*(Fosc))/(4*Pre)-1</f>
+        <f>((Tpwm)*(Fosc*1000000))/(4*Pre)-1</f>
         <v>124</v>
       </c>
       <c r="D7" s="14">
-        <f>IF((LOG10(Fosc/(Fpwm/1000)))/(LOG10(2))&gt;10,10,(LOG10(Fosc/(Fpwm/1000)))/(LOG10(2)))</f>
+        <f>IF((LOG10(Fosc*1000000/(Fpwm)))/(LOG10(2))&gt;10,10,(LOG10(Fosc*1000000/(Fpwm)))/(LOG10(2)))</f>
         <v>10</v>
       </c>
       <c r="E7" s="15">
-        <f>(Duty*Tpwm*Fosc)/(Pre)</f>
-        <v>250</v>
+        <f>(Duty*Tpwm*Fosc*1000000)/(Pre)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -1018,7 +1035,7 @@
       <c r="D10" s="32"/>
       <c r="E10" s="33"/>
       <c r="G10" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1026,13 +1043,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1044,54 +1061,104 @@
         <v>4.9999999999999998E-7</v>
       </c>
       <c r="D12" s="9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E12" s="18">
-        <v>2000</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <f>1/E12</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1.0416666666666667E-4</v>
       </c>
       <c r="C14" s="26">
         <f>(_xlfn.BITLSHIFT(1,E14))-(B14)/(C12*D12)</f>
-        <v>64536</v>
+        <v>229.95833333333334</v>
       </c>
       <c r="E14" s="18">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="36"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="23">
+        <v>8</v>
+      </c>
+      <c r="C19" s="9">
+        <v>16</v>
+      </c>
+      <c r="D19" s="18">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="8">
+        <f>1/D19</f>
+        <v>1.0416666666666667E-4</v>
+      </c>
+      <c r="C21" s="26">
+        <f>((B21)*(B19*1000000))/(4*C19)-1</f>
+        <v>12.020833333333334</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1870,29 +1937,37 @@
     <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B9:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notBetween">
+      <formula>0</formula>
+      <formula>255</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
       <formula>0</formula>
       <formula>255</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+  <conditionalFormatting sqref="C21">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
       <formula>0</formula>
       <formula>255</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C5 C19" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,4,16"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="B5 B12" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="B5 B12 B19" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D12" xr:uid="{5825D9D1-57B3-4C3C-A12F-8A11388FAA98}">

</xml_diff>

<commit_message>
Practica 5: Protipo de transmision
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Microcontroladores_PIC\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3215DC58-BFEF-4DF0-858B-0C2617B9E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFCAAA4-2B0C-455B-ABDD-9EA2D273B279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -650,6 +650,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -662,22 +677,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -944,20 +943,20 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
@@ -1020,20 +1019,20 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
       <c r="G10" s="20" t="s">
         <v>12</v>
       </c>
@@ -1093,22 +1092,21 @@
     </row>
     <row r="15" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="27"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="31" t="s">
+    <row r="17" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="36"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
         <v>1</v>
       </c>
@@ -1119,7 +1117,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="23">
         <v>8</v>
       </c>
@@ -1130,7 +1128,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>14</v>
       </c>
@@ -1138,7 +1136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8">
         <f>1/D19</f>
         <v>1.0416666666666667E-4</v>
@@ -1148,17 +1146,17 @@
         <v>12.020833333333334</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Practica 5: Version Final
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Microcontroladores_PIC\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFCAAA4-2B0C-455B-ABDD-9EA2D273B279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D4E58D-B508-4431-A6A9-F861AC5555A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1060,7 @@
         <v>4.9999999999999998E-7</v>
       </c>
       <c r="D12" s="9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E12" s="18">
         <v>9600</v>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="C14" s="26">
         <f>(_xlfn.BITLSHIFT(1,E14))-(B14)/(C12*D12)</f>
-        <v>229.95833333333334</v>
+        <v>47.666666666666657</v>
       </c>
       <c r="E14" s="18">
         <v>8</v>
@@ -1125,7 +1125,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="18">
-        <v>9600</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1139,11 +1139,11 @@
     <row r="21" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8">
         <f>1/D19</f>
-        <v>1.0416666666666667E-4</v>
+        <v>4.1666666666666669E-4</v>
       </c>
       <c r="C21" s="26">
         <f>((B21)*(B19*1000000))/(4*C19)-1</f>
-        <v>12.020833333333334</v>
+        <v>51.083333333333336</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Practica 7: Impresion en GLCD
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Microcontroladores_PIC\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D4E58D-B508-4431-A6A9-F861AC5555A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1621F24D-8DF7-4743-8F9A-5A99592D9408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>SE CONOCEN ESTOS DATOS</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Pre-escaler Timer 0</t>
-  </si>
-  <si>
-    <t>Quiero una señal de 1 kHz</t>
   </si>
   <si>
     <t>Frecuencia (Hz)</t>
@@ -926,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -966,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>6</v>
@@ -974,7 +971,7 @@
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C5" s="9">
         <v>16</v>
@@ -983,7 +980,7 @@
         <v>1000</v>
       </c>
       <c r="E5" s="11">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1007,7 +1004,7 @@
       </c>
       <c r="C7" s="2">
         <f>((Tpwm)*(Fosc*1000000))/(4*Pre)-1</f>
-        <v>124</v>
+        <v>249</v>
       </c>
       <c r="D7" s="14">
         <f>IF((LOG10(Fosc*1000000/(Fpwm)))/(LOG10(2))&gt;10,10,(LOG10(Fosc*1000000/(Fpwm)))/(LOG10(2)))</f>
@@ -1015,7 +1012,7 @@
       </c>
       <c r="E7" s="15">
         <f>(Duty*Tpwm*Fosc*1000000)/(Pre)</f>
-        <v>0</v>
+        <v>750</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
@@ -1033,22 +1030,20 @@
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="30"/>
-      <c r="G10" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1060,40 +1055,40 @@
         <v>4.9999999999999998E-7</v>
       </c>
       <c r="D12" s="9">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E12" s="18">
-        <v>9600</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <f>1/E12</f>
-        <v>1.0416666666666667E-4</v>
+        <v>0.2</v>
       </c>
       <c r="C14" s="26">
-        <f>(_xlfn.BITLSHIFT(1,E14))-(B14)/(C12*D12)</f>
-        <v>47.666666666666657</v>
+        <f>(_xlfn.BITLSHIFT(1,E14)-1)-(B14)/(C12*D12)</f>
+        <v>53035</v>
       </c>
       <c r="E14" s="18">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -1114,23 +1109,23 @@
         <v>11</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="23">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C19" s="9">
         <v>16</v>
       </c>
       <c r="D19" s="18">
-        <v>2400</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>3</v>
@@ -1139,11 +1134,11 @@
     <row r="21" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8">
         <f>1/D19</f>
-        <v>4.1666666666666669E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C21" s="26">
         <f>((B21)*(B19*1000000))/(4*C19)-1</f>
-        <v>51.083333333333336</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1952,7 +1947,7 @@
   <conditionalFormatting sqref="C14">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
       <formula>0</formula>
-      <formula>255</formula>
+      <formula>_xlfn.BITLSHIFT(1,E14) - 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">

</xml_diff>

<commit_message>
Practica 7: Elementos e impresion
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Microcontroladores_PIC\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1621F24D-8DF7-4743-8F9A-5A99592D9408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A8E1A2-75BC-418E-AA6F-D35A8719DBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1055,10 +1055,10 @@
         <v>4.9999999999999998E-7</v>
       </c>
       <c r="D12" s="9">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E12" s="18">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1075,11 +1075,11 @@
     <row r="14" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <f>1/E12</f>
-        <v>0.2</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="C14" s="26">
         <f>(_xlfn.BITLSHIFT(1,E14)-1)-(B14)/(C12*D12)</f>
-        <v>53035</v>
+        <v>48868.333333333328</v>
       </c>
       <c r="E14" s="18">
         <v>16</v>

</xml_diff>

<commit_message>
Practica 7: Videojuego version final
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Microcontroladores_PIC\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A8E1A2-75BC-418E-AA6F-D35A8719DBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BBF3AC-A8F0-494D-962E-EB2F31A79C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1048,17 +1048,17 @@
     </row>
     <row r="12" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C12" s="22">
         <f>4/(B12*1000000)</f>
-        <v>4.9999999999999998E-7</v>
+        <v>8.3333333333333338E-8</v>
       </c>
       <c r="D12" s="9">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E12" s="18">
-        <v>60</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1075,11 +1075,11 @@
     <row r="14" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <f>1/E12</f>
-        <v>1.6666666666666666E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C14" s="26">
         <f>(_xlfn.BITLSHIFT(1,E14)-1)-(B14)/(C12*D12)</f>
-        <v>48868.333333333328</v>
+        <v>18660</v>
       </c>
       <c r="E14" s="18">
         <v>16</v>

</xml_diff>

<commit_message>
SCADA: Inicio y avance de programacion
</commit_message>
<xml_diff>
--- a/Recursos/Calculos PWM.xlsx
+++ b/Recursos/Calculos PWM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Microcontroladores_PIC\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BBF3AC-A8F0-494D-962E-EB2F31A79C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67D2D66-95C0-4DC0-BDEE-BA632FE81BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="30" yWindow="750" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -924,7 +924,7 @@
   <dimension ref="B1:G809"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="205" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -974,13 +974,13 @@
         <v>16</v>
       </c>
       <c r="C5" s="9">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D5" s="9">
-        <v>1000</v>
+        <v>200000</v>
       </c>
       <c r="E5" s="11">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1000,19 +1000,19 @@
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <f>1/Fpwm</f>
-        <v>1E-3</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="C7" s="2">
         <f>((Tpwm)*(Fosc*1000000))/(4*Pre)-1</f>
-        <v>249</v>
+        <v>19</v>
       </c>
       <c r="D7" s="14">
         <f>IF((LOG10(Fosc*1000000/(Fpwm)))/(LOG10(2))&gt;10,10,(LOG10(Fosc*1000000/(Fpwm)))/(LOG10(2)))</f>
-        <v>10</v>
+        <v>6.3219280948873617</v>
       </c>
       <c r="E7" s="15">
         <f>(Duty*Tpwm*Fosc*1000000)/(Pre)</f>
-        <v>750</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
@@ -1048,17 +1048,17 @@
     </row>
     <row r="12" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C12" s="22">
         <f>4/(B12*1000000)</f>
-        <v>8.3333333333333338E-8</v>
+        <v>1.9999999999999999E-7</v>
       </c>
       <c r="D12" s="9">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E12" s="18">
-        <v>16</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1075,18 +1075,18 @@
     <row r="14" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <f>1/E12</f>
-        <v>6.25E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="C14" s="26">
         <f>(_xlfn.BITLSHIFT(1,E14)-1)-(B14)/(C12*D12)</f>
-        <v>18660</v>
+        <v>98.75</v>
       </c>
       <c r="E14" s="18">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="31" t="s">
         <v>17</v>
       </c>
@@ -1094,14 +1094,18 @@
       <c r="D16" s="31"/>
       <c r="E16" s="27"/>
     </row>
-    <row r="17" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="30"/>
+      <c r="E17">
+        <f>1/E18</f>
+        <v>610.3515625</v>
+      </c>
     </row>
-    <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
         <v>1</v>
       </c>
@@ -1111,19 +1115,23 @@
       <c r="D18" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="E18">
+        <f>4/(B12*1000000)*_xlfn.BITLSHIFT(1,E14)*D12</f>
+        <v>1.6383999999999999E-3</v>
+      </c>
     </row>
-    <row r="19" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="23">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C19" s="9">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D19" s="18">
-        <v>1000</v>
+        <v>500000</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>13</v>
       </c>
@@ -1131,27 +1139,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8">
         <f>1/D19</f>
-        <v>1E-3</v>
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="C21" s="26">
         <f>((B21)*(B19*1000000))/(4*C19)-1</f>
-        <v>249</v>
+        <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>